<commit_message>
Adicionando workflow para publicar imagem no dockehub
</commit_message>
<xml_diff>
--- a/python/scripts/metadado.xlsx
+++ b/python/scripts/metadado.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/6f054485a52af266/Impacta/DE04/dataops/de04_dataops/aula02/scripts/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Arch\mnt\wsl\Projects\Mba\DataOpsDevelopDeliverAnalytics\de04_dataops\python\scripts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="72" documentId="11_AD4D361C20488DEA4E38A0B7F41969B45ADEDD8B" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8A8F9203-BC21-47CF-A020-10B26CA3D996}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FC676EF-FEEC-45F2-9AF7-760563EF2F3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4080" yWindow="2985" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-25710" yWindow="-110" windowWidth="25820" windowHeight="14620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Plan1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="38">
   <si>
     <t>tabela</t>
   </si>
@@ -124,6 +124,21 @@
   </si>
   <si>
     <t>dob.date</t>
+  </si>
+  <si>
+    <t>tratamento</t>
+  </si>
+  <si>
+    <t>lowercase</t>
+  </si>
+  <si>
+    <t>n/a</t>
+  </si>
+  <si>
+    <t>remover caracteres especiais</t>
+  </si>
+  <si>
+    <t>formatar para Y-m-d</t>
   </si>
 </sst>
 </file>
@@ -465,21 +480,21 @@
   <dimension ref="A1:L26"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:O10"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.85546875" customWidth="1"/>
-    <col min="5" max="5" width="33.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.5703125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="11.28515625" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.26953125" customWidth="1"/>
+    <col min="4" max="4" width="26.81640625" customWidth="1"/>
+    <col min="5" max="5" width="33.453125" customWidth="1"/>
+    <col min="8" max="8" width="25.1796875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="11.26953125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -501,13 +516,15 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="1" t="s">
+        <v>33</v>
+      </c>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
       <c r="K1" s="1"/>
       <c r="L1" s="1"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>22</v>
       </c>
@@ -529,8 +546,11 @@
       <c r="G2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>22</v>
       </c>
@@ -552,8 +572,11 @@
       <c r="G3">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H3" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>22</v>
       </c>
@@ -575,8 +598,11 @@
       <c r="G4">
         <v>1</v>
       </c>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>22</v>
       </c>
@@ -598,8 +624,11 @@
       <c r="G5">
         <v>0</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>22</v>
       </c>
@@ -621,8 +650,11 @@
       <c r="G6">
         <v>0</v>
       </c>
-    </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>22</v>
       </c>
@@ -644,8 +676,11 @@
       <c r="G7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H7" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -667,8 +702,11 @@
       <c r="G8">
         <v>0</v>
       </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H8" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>22</v>
       </c>
@@ -690,8 +728,11 @@
       <c r="G9">
         <v>1</v>
       </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="H9" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>22</v>
       </c>
@@ -713,11 +754,15 @@
       <c r="G10">
         <v>1</v>
       </c>
-    </row>
-    <row r="26" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="26" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H26" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>